<commit_message>
Updated bal - tentative
</commit_message>
<xml_diff>
--- a/Housekeeping/Balance.xlsx
+++ b/Housekeeping/Balance.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="45" windowWidth="15135" windowHeight="8130"/>
+    <workbookView xWindow="120" yWindow="45" windowWidth="15135" windowHeight="8130" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="114210"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
   <si>
     <t>Date</t>
   </si>
@@ -55,13 +55,40 @@
   </si>
   <si>
     <t>Limits</t>
+  </si>
+  <si>
+    <t>5/13/2014</t>
+  </si>
+  <si>
+    <t>13-05-2014</t>
+  </si>
+  <si>
+    <t>EQ</t>
+  </si>
+  <si>
+    <t>FO</t>
+  </si>
+  <si>
+    <t>PL</t>
+  </si>
+  <si>
+    <t>NX</t>
+  </si>
+  <si>
+    <t>Tot</t>
+  </si>
+  <si>
+    <t>Com</t>
+  </si>
+  <si>
+    <t>APL</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -70,12 +97,22 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -98,12 +135,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -117,6 +153,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -411,23 +458,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.28515625" customWidth="1"/>
+    <col min="1" max="1" width="14.28515625" style="3" customWidth="1"/>
     <col min="2" max="2" width="16.28515625" customWidth="1"/>
     <col min="3" max="3" width="15.85546875" customWidth="1"/>
     <col min="4" max="4" width="20.5703125" customWidth="1"/>
     <col min="5" max="5" width="17.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" t="s">
+    <row r="1" spans="1:5" s="8" customFormat="1">
+      <c r="A1" s="8" t="s">
         <v>12</v>
       </c>
     </row>
@@ -449,7 +496,7 @@
       </c>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="2">
+      <c r="A5" s="7">
         <v>41887</v>
       </c>
       <c r="E5">
@@ -457,10 +504,10 @@
       </c>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="2">
+      <c r="A6" s="7">
         <v>41978</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="2">
         <v>-32255.919999999998</v>
       </c>
       <c r="E6">
@@ -468,7 +515,13 @@
         <v>525268.78999999992</v>
       </c>
     </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="0" r:id="rId1"/>
 </worksheet>
@@ -476,112 +529,154 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="6" max="6" width="15.7109375" style="4" customWidth="1"/>
+    <col min="6" max="6" width="15.7109375" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
-      <c r="A3">
+    <row r="3" spans="1:9" s="11" customFormat="1">
+      <c r="A3" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="I3" s="11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5">
         <v>10182.74</v>
       </c>
-      <c r="B3">
+      <c r="B5">
         <v>418730.31</v>
       </c>
-      <c r="E3">
-        <f>SUM(A3:D3)</f>
+      <c r="E5">
+        <f>SUM(A5:D5)</f>
         <v>428913.05</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F5" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
-      <c r="C4">
+    <row r="6" spans="1:9">
+      <c r="C6">
         <v>7008.24</v>
       </c>
-      <c r="E4">
-        <f>SUM(E3,C4:D4)</f>
+      <c r="E6">
+        <f t="shared" ref="E6:E11" si="0">SUM(E5,C6:D6)</f>
         <v>435921.29</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="F6" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
-      <c r="C5">
+    <row r="7" spans="1:9">
+      <c r="C7">
         <v>3191.13</v>
       </c>
-      <c r="E5">
-        <f>SUM(E4,C5:D5)</f>
+      <c r="E7">
+        <f t="shared" si="0"/>
         <v>439112.42</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="F7" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
-      <c r="C6">
+    <row r="8" spans="1:9">
+      <c r="C8">
         <v>-1587.71</v>
       </c>
-      <c r="E6">
-        <f>SUM(E5,C6:D6)</f>
+      <c r="E8">
+        <f t="shared" si="0"/>
         <v>437524.70999999996</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="F8" s="5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
-      <c r="D7">
+    <row r="9" spans="1:9">
+      <c r="D9">
         <v>50000</v>
       </c>
-      <c r="E7">
-        <f>SUM(E6,C7:D7)</f>
+      <c r="E9">
+        <f t="shared" si="0"/>
         <v>487524.70999999996</v>
       </c>
-      <c r="F7" s="7" t="s">
+      <c r="F9" s="6" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
-      <c r="D8">
+    <row r="10" spans="1:9">
+      <c r="D10">
         <v>45000</v>
       </c>
-      <c r="E8">
-        <f>SUM(E7,C8:D8)</f>
+      <c r="E10">
+        <f t="shared" si="0"/>
         <v>532524.71</v>
       </c>
-      <c r="F8" s="7" t="s">
+      <c r="F10" s="6" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
-      <c r="C9">
+    <row r="11" spans="1:9">
+      <c r="C11">
         <v>-32255.919999999998</v>
       </c>
-      <c r="D9">
+      <c r="D11">
         <v>20000</v>
       </c>
-      <c r="E9">
-        <f>SUM(E8,C9:D9)</f>
+      <c r="E11">
+        <f t="shared" si="0"/>
         <v>520268.79</v>
       </c>
-      <c r="F9" s="7" t="s">
+      <c r="F11" s="6" t="s">
         <v>10</v>
       </c>
     </row>
+    <row r="12" spans="1:9">
+      <c r="D12">
+        <v>30000</v>
+      </c>
+      <c r="E12">
+        <f>SUM(E11,C12:D12)</f>
+        <v>550268.79</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="I12">
+        <v>-9000</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -593,6 +688,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated till 23-05-2014 and Rel stuff
</commit_message>
<xml_diff>
--- a/Housekeeping/Balance.xlsx
+++ b/Housekeeping/Balance.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
   <si>
     <t>Date</t>
   </si>
@@ -100,6 +100,9 @@
   </si>
   <si>
     <t>19-05-2014</t>
+  </si>
+  <si>
+    <t>23-05-2014</t>
   </si>
 </sst>
 </file>
@@ -546,10 +549,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I18"/>
+  <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -766,6 +769,18 @@
         <v>24</v>
       </c>
       <c r="I18" s="9"/>
+    </row>
+    <row r="19" spans="3:9">
+      <c r="C19">
+        <v>-101334.85</v>
+      </c>
+      <c r="E19" s="10">
+        <f>SUM(E18,I19,C19,D19)</f>
+        <v>413413.98999999987</v>
+      </c>
+      <c r="F19" s="6" t="s">
+        <v>28</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>